<commit_message>
specify 23 bp core region for search target
</commit_message>
<xml_diff>
--- a/TEMPLATE_orderingConfig.xlsx
+++ b/TEMPLATE_orderingConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi.bhattaraikline\Shipman_Lab_Dev\Spacer-Seq\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6A8C03-205C-490C-B9BA-1609E9E075D7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A061CC-B62C-44CA-9827-0527A9B1FAA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7070" xr2:uid="{5A187682-41C2-44FD-95C2-5AD1F8E09DAA}"/>
   </bookViews>
@@ -30,15 +30,6 @@
     <t>Sample ID</t>
   </si>
   <si>
-    <t>Spacer "A"</t>
-  </si>
-  <si>
-    <t>Spacer "B"</t>
-  </si>
-  <si>
-    <t>Spacer "C"</t>
-  </si>
-  <si>
     <t>msSBK_3_37</t>
   </si>
   <si>
@@ -49,6 +40,15 @@
   </si>
   <si>
     <t>&lt;--- Example. Replace this row</t>
+  </si>
+  <si>
+    <t>Spacer "A" (23 base core)</t>
+  </si>
+  <si>
+    <t>Spacer "B" (23 base core)</t>
+  </si>
+  <si>
+    <t>Spacer "C" (23 base core)</t>
   </si>
 </sst>
 </file>
@@ -412,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FADEC9AC-0EED-4505-9985-7F0BE00C7BDB}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -428,30 +428,30 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>